<commit_message>
Renamed the PLL1 device to `PLL1_1`.
</commit_message>
<xml_diff>
--- a/andes/cases/ieee14/ieee14_regcp1.xlsx
+++ b/andes/cases/ieee14/ieee14_regcp1.xlsx
@@ -1462,7 +1462,7 @@
         <v>1</v>
       </c>
       <c r="Y2" t="str">
-        <v>PLL1_2</v>
+        <v>PLL1_1</v>
       </c>
     </row>
   </sheetData>
@@ -2110,13 +2110,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="str">
-        <v>PLL1_2</v>
+        <v>PLL1_1</v>
       </c>
       <c r="C2" t="str">
         <v>1</v>
       </c>
       <c r="D2" t="str">
-        <v>PLL1_2</v>
+        <v>PLL1_1</v>
       </c>
       <c r="E2" t="str">
         <v>8</v>

</xml_diff>